<commit_message>
endpoint check + page sweep smoke test for category pages
</commit_message>
<xml_diff>
--- a/Data Files/prodLog.xlsx
+++ b/Data Files/prodLog.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zsmith\Desktop\katalon_lexc\katalon_lexc_global\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView windowHeight="6465" windowWidth="25980" xWindow="0" yWindow="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25980" windowHeight="6465"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" r:id="rId1" sheetId="1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="28">
   <si>
     <t>build</t>
   </si>
@@ -43,13 +43,79 @@
   </si>
   <si>
     <t>default</t>
+  </si>
+  <si>
+    <t>CategoryPages</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fe11f8d1ec built at 2020-09-10 13:02
+</t>
+  </si>
+  <si>
+    <t>ComparePages</t>
+  </si>
+  <si>
+    <t>DealerPages</t>
+  </si>
+  <si>
+    <t>ErrorPages</t>
+  </si>
+  <si>
+    <t>FCVPages</t>
+  </si>
+  <si>
+    <t>HomeOffersPages</t>
+  </si>
+  <si>
+    <t>LCertifiedPages</t>
+  </si>
+  <si>
+    <t>MiscPages</t>
+  </si>
+  <si>
+    <t>ModelPagesAccessories</t>
+  </si>
+  <si>
+    <t>ModelPagesDesign</t>
+  </si>
+  <si>
+    <t>ModelPagesFeatures</t>
+  </si>
+  <si>
+    <t>ModelPagesGallery</t>
+  </si>
+  <si>
+    <t>ModelPagesOffers</t>
+  </si>
+  <si>
+    <t>ModelPagesOverview</t>
+  </si>
+  <si>
+    <t>ModelPagesOwners</t>
+  </si>
+  <si>
+    <t>ModelPagesPackages</t>
+  </si>
+  <si>
+    <t>ModelPagesPerformance</t>
+  </si>
+  <si>
+    <t>ModelPagesSafety</t>
+  </si>
+  <si>
+    <t>ModelPagesSpecifications</t>
+  </si>
+  <si>
+    <t>ModelPagesTechnology</t>
+  </si>
+  <si>
+    <t>SponsoredAthletes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -77,16 +143,16 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -103,10 +169,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -141,7 +207,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -176,7 +242,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -270,21 +336,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -301,7 +367,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -353,18 +419,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A4" sqref="A4:B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -393,7 +459,175 @@
         <v>4</v>
       </c>
     </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>1</v>
+      </c>
+      <c r="B24" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
version-triggered smoke test created for all categories
</commit_message>
<xml_diff>
--- a/Data Files/prodLog.xlsx
+++ b/Data Files/prodLog.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zsmith\Desktop\katalon_lexc\katalon_lexc_global\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25980" windowHeight="6465"/>
+    <workbookView windowHeight="6465" windowWidth="25980" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" r:id="rId1" sheetId="1"/>
   </sheets>
   <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="28">
   <si>
     <t>build</t>
   </si>
@@ -116,6 +116,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -143,16 +144,16 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -169,10 +170,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -207,7 +208,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -242,7 +243,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -336,21 +337,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -367,7 +368,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -419,18 +420,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:B24"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -469,7 +470,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
         <v>8</v>
@@ -525,7 +526,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B12" t="s">
         <v>15</v>
@@ -613,7 +614,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B23" t="s">
         <v>26</v>
@@ -621,13 +622,13 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B24" t="s">
         <v>27</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated CICT test suites
</commit_message>
<xml_diff>
--- a/Data Files/prodLog.xlsx
+++ b/Data Files/prodLog.xlsx
@@ -48,68 +48,68 @@
     <t>CategoryPages</t>
   </si>
   <si>
+    <t>ComparePages</t>
+  </si>
+  <si>
+    <t>DealerPages</t>
+  </si>
+  <si>
+    <t>ErrorPages</t>
+  </si>
+  <si>
+    <t>FCVPages</t>
+  </si>
+  <si>
+    <t>HomeOffersPages</t>
+  </si>
+  <si>
+    <t>LCertifiedPages</t>
+  </si>
+  <si>
+    <t>MiscPages</t>
+  </si>
+  <si>
+    <t>ModelPagesAccessories</t>
+  </si>
+  <si>
+    <t>ModelPagesDesign</t>
+  </si>
+  <si>
+    <t>ModelPagesFeatures</t>
+  </si>
+  <si>
+    <t>ModelPagesGallery</t>
+  </si>
+  <si>
+    <t>ModelPagesOffers</t>
+  </si>
+  <si>
+    <t>ModelPagesOverview</t>
+  </si>
+  <si>
+    <t>ModelPagesOwners</t>
+  </si>
+  <si>
+    <t>ModelPagesPackages</t>
+  </si>
+  <si>
+    <t>ModelPagesPerformance</t>
+  </si>
+  <si>
+    <t>ModelPagesSafety</t>
+  </si>
+  <si>
+    <t>ModelPagesSpecifications</t>
+  </si>
+  <si>
+    <t>ModelPagesTechnology</t>
+  </si>
+  <si>
+    <t>SponsoredAthletes</t>
+  </si>
+  <si>
     <t xml:space="preserve">fe11f8d1ec built at 2020-09-10 13:02
 </t>
-  </si>
-  <si>
-    <t>ComparePages</t>
-  </si>
-  <si>
-    <t>DealerPages</t>
-  </si>
-  <si>
-    <t>ErrorPages</t>
-  </si>
-  <si>
-    <t>FCVPages</t>
-  </si>
-  <si>
-    <t>HomeOffersPages</t>
-  </si>
-  <si>
-    <t>LCertifiedPages</t>
-  </si>
-  <si>
-    <t>MiscPages</t>
-  </si>
-  <si>
-    <t>ModelPagesAccessories</t>
-  </si>
-  <si>
-    <t>ModelPagesDesign</t>
-  </si>
-  <si>
-    <t>ModelPagesFeatures</t>
-  </si>
-  <si>
-    <t>ModelPagesGallery</t>
-  </si>
-  <si>
-    <t>ModelPagesOffers</t>
-  </si>
-  <si>
-    <t>ModelPagesOverview</t>
-  </si>
-  <si>
-    <t>ModelPagesOwners</t>
-  </si>
-  <si>
-    <t>ModelPagesPackages</t>
-  </si>
-  <si>
-    <t>ModelPagesPerformance</t>
-  </si>
-  <si>
-    <t>ModelPagesSafety</t>
-  </si>
-  <si>
-    <t>ModelPagesSpecifications</t>
-  </si>
-  <si>
-    <t>ModelPagesTechnology</t>
-  </si>
-  <si>
-    <t>SponsoredAthletes</t>
   </si>
 </sst>
 </file>
@@ -431,7 +431,7 @@
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -462,7 +462,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -470,10 +470,10 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
         <v>7</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -481,7 +481,7 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -489,7 +489,7 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -497,7 +497,7 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -505,7 +505,7 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -513,7 +513,7 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -521,15 +521,15 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -537,7 +537,7 @@
         <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -545,7 +545,7 @@
         <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -553,7 +553,7 @@
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -561,7 +561,7 @@
         <v>1</v>
       </c>
       <c r="B16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -569,7 +569,7 @@
         <v>1</v>
       </c>
       <c r="B17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -577,7 +577,7 @@
         <v>1</v>
       </c>
       <c r="B18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -585,7 +585,7 @@
         <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -593,7 +593,7 @@
         <v>1</v>
       </c>
       <c r="B20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -601,7 +601,7 @@
         <v>1</v>
       </c>
       <c r="B21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -609,23 +609,23 @@
         <v>1</v>
       </c>
       <c r="B22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="B23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="B24" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>